<commit_message>
Refactoring, incorporated genome-length SRLV sequences from after 2017. Rebuilt trees
</commit_message>
<xml_diff>
--- a/tabular/extension/srlv-curated.xlsx
+++ b/tabular/extension/srlv-curated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Lentivirus-GLUE/tabular/extension/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F5286C-3116-AB47-B807-7FE551908FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B68284-5E0D-C446-954B-F5573F61198A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16680" yWindow="5440" windowWidth="28060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5344" uniqueCount="1247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5557" uniqueCount="1296">
   <si>
     <t>Number</t>
   </si>
@@ -3770,6 +3770,153 @@
   </si>
   <si>
     <t>AY101611_U64439</t>
+  </si>
+  <si>
+    <t>MT993918</t>
+  </si>
+  <si>
+    <t>MT993917</t>
+  </si>
+  <si>
+    <t>MT993916</t>
+  </si>
+  <si>
+    <t>MT993915</t>
+  </si>
+  <si>
+    <t>MT993914</t>
+  </si>
+  <si>
+    <t>MT993913</t>
+  </si>
+  <si>
+    <t>MT993912</t>
+  </si>
+  <si>
+    <t>MT993911</t>
+  </si>
+  <si>
+    <t>MT993910</t>
+  </si>
+  <si>
+    <t>MT993909</t>
+  </si>
+  <si>
+    <t>MT993908</t>
+  </si>
+  <si>
+    <t>MT993907</t>
+  </si>
+  <si>
+    <t>MT993906</t>
+  </si>
+  <si>
+    <t>MT993905</t>
+  </si>
+  <si>
+    <t>MT993904</t>
+  </si>
+  <si>
+    <t>MT993903</t>
+  </si>
+  <si>
+    <t>MT993902</t>
+  </si>
+  <si>
+    <t>MT993901</t>
+  </si>
+  <si>
+    <t>MT993900</t>
+  </si>
+  <si>
+    <t>MT993899</t>
+  </si>
+  <si>
+    <t>MT993898</t>
+  </si>
+  <si>
+    <t>MT993897</t>
+  </si>
+  <si>
+    <t>MT993896</t>
+  </si>
+  <si>
+    <t>MG554414</t>
+  </si>
+  <si>
+    <t>MG554413</t>
+  </si>
+  <si>
+    <t>MG554412</t>
+  </si>
+  <si>
+    <t>MG554411</t>
+  </si>
+  <si>
+    <t>MG554410</t>
+  </si>
+  <si>
+    <t>MG554409</t>
+  </si>
+  <si>
+    <t>MG554408</t>
+  </si>
+  <si>
+    <t>MG554407</t>
+  </si>
+  <si>
+    <t>MG554406</t>
+  </si>
+  <si>
+    <t>MG554405</t>
+  </si>
+  <si>
+    <t>MG554404</t>
+  </si>
+  <si>
+    <t>MG554403</t>
+  </si>
+  <si>
+    <t>MG554402</t>
+  </si>
+  <si>
+    <t>MH374291</t>
+  </si>
+  <si>
+    <t>MH374290</t>
+  </si>
+  <si>
+    <t>MH374289</t>
+  </si>
+  <si>
+    <t>MH374288</t>
+  </si>
+  <si>
+    <t>MH374287</t>
+  </si>
+  <si>
+    <t>MH374286</t>
+  </si>
+  <si>
+    <t>MH374285</t>
+  </si>
+  <si>
+    <t>MH374284</t>
+  </si>
+  <si>
+    <t>MH374283</t>
+  </si>
+  <si>
+    <t>MH936675</t>
+  </si>
+  <si>
+    <t>MH936674</t>
+  </si>
+  <si>
+    <t>MG996440</t>
+  </si>
+  <si>
+    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -4234,10 +4381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L675"/>
+  <dimension ref="A1:L723"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A654" workbookViewId="0">
-      <selection activeCell="J666" sqref="A1:L675"/>
+    <sheetView tabSelected="1" topLeftCell="A671" workbookViewId="0">
+      <selection activeCell="I697" sqref="I697"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29892,6 +30039,741 @@
       </c>
       <c r="L675" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="676" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B676" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C676" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D676" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G676" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K676" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L676" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="677" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B677" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C677" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D677" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G677" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K677" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L677" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="678" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B678" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C678" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D678" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G678" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K678" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L678" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="679" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B679" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C679" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D679" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G679" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K679" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L679" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="680" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B680" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C680" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D680" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G680" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K680" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L680" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="681" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B681" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C681" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D681" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G681" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K681" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L681" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="682" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B682" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C682" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D682" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G682" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K682" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L682" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="683" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B683" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C683" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D683" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G683" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K683" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L683" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="684" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B684" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C684" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D684" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G684" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K684" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L684" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="685" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B685" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C685" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D685" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G685" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K685" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L685" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="686" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B686" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C686" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D686" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G686" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K686" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L686" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="687" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B687" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C687" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D687" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G687" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K687" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L687" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="688" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B688" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C688" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D688" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G688" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K688" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L688" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="689" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B689" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C689" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D689" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G689" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K689" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L689" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="690" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B690" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C690" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D690" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G690" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K690" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L690" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="691" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B691" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C691" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D691" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G691" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K691" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L691" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="692" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B692" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C692" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D692" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G692" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K692" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L692" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="693" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B693" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C693" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D693" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G693" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K693" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L693" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="694" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B694" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C694" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D694" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G694" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K694" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L694" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="695" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B695" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C695" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D695" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G695" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K695" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L695" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="696" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B696" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C696" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D696" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G696" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K696" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L696" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="697" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B697" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C697" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D697" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G697" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K697" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L697" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="698" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B698" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C698" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D698" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="G698" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K698" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L698" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="699" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B699" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C699" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K699" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="700" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B700" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C700" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K700" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="701" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B701" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C701" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K701" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="702" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B702" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C702" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K702" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="703" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B703" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C703" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K703" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="704" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B704" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C704" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K704" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="705" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B705" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C705" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K705" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="706" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B706" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C706" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K706" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="707" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B707" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C707" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K707" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="708" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B708" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C708" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K708" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="709" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B709" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C709" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K709" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="710" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B710" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C710" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K710" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="711" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B711" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C711" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K711" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="712" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B712" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C712" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K712" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="713" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B713" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C713" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K713" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="714" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B714" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C714" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K714" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="715" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B715" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C715" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K715" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="716" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B716" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C716" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K716" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="717" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B717" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C717" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K717" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="718" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B718" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C718" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K718" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="719" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B719" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C719" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K719" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="720" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B720" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C720" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K720" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="721" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B721" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C721" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K721" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="722" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B722" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C722" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K722" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="723" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B723" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C723" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K723" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>